<commit_message>
Add support for importing data without keys Add support for importing data and automatically create destination table Add test for Post-execute-SQL Make meta query function static methods
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -494,320 +494,320 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>7369</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>9</v>
       </c>
-      <c r="D2" t="n">
+      <c t="n" r="D2">
         <v>7902</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>10</v>
       </c>
-      <c r="F2" t="n">
+      <c t="n" r="F2">
         <v>800</v>
       </c>
-      <c r="G2" t="s"/>
-      <c r="H2" t="n">
+      <c t="s" r="G2"/>
+      <c t="n" r="H2">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="n">
+      <c t="n" r="A3">
         <v>7499</v>
       </c>
-      <c r="B3" t="s">
+      <c t="s" r="B3">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c t="s" r="C3">
         <v>12</v>
       </c>
-      <c r="D3" t="n">
+      <c t="n" r="D3">
         <v>7698</v>
       </c>
-      <c r="E3" t="s">
+      <c t="s" r="E3">
         <v>13</v>
       </c>
-      <c r="F3" t="n">
+      <c t="n" r="F3">
         <v>1600</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>300</v>
       </c>
-      <c r="H3" t="n">
+      <c t="n" r="H3">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="n">
+      <c t="n" r="A4">
         <v>7521</v>
       </c>
-      <c r="B4" t="s">
+      <c t="s" r="B4">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c t="s" r="C4">
         <v>15</v>
       </c>
-      <c r="D4" t="n">
+      <c t="n" r="D4">
         <v>7698</v>
       </c>
-      <c r="E4" t="s">
+      <c t="s" r="E4">
         <v>16</v>
       </c>
-      <c r="F4" t="n">
+      <c t="n" r="F4">
         <v>1250</v>
       </c>
-      <c r="G4" t="n">
+      <c t="n" r="G4">
         <v>500</v>
       </c>
-      <c r="H4" t="n">
+      <c t="n" r="H4">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="n">
+      <c t="n" r="A5">
         <v>7566</v>
       </c>
-      <c r="B5" t="s">
+      <c t="s" r="B5">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c t="s" r="C5">
         <v>18</v>
       </c>
-      <c r="D5" t="n">
+      <c t="n" r="D5">
         <v>7839</v>
       </c>
-      <c r="E5" t="s">
+      <c t="s" r="E5">
         <v>19</v>
       </c>
-      <c r="F5" t="n">
+      <c t="n" r="F5">
         <v>2975</v>
       </c>
-      <c r="G5" t="s"/>
-      <c r="H5" t="n">
+      <c t="s" r="G5"/>
+      <c t="n" r="H5">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="n">
+      <c t="n" r="A6">
         <v>7654</v>
       </c>
-      <c r="B6" t="s">
+      <c t="s" r="B6">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c t="s" r="C6">
         <v>15</v>
       </c>
-      <c r="D6" t="n">
+      <c t="n" r="D6">
         <v>7698</v>
       </c>
-      <c r="E6" t="s">
+      <c t="s" r="E6">
         <v>21</v>
       </c>
-      <c r="F6" t="n">
+      <c t="n" r="F6">
         <v>1250</v>
       </c>
-      <c r="G6" t="n">
+      <c t="n" r="G6">
         <v>1400</v>
       </c>
-      <c r="H6" t="n">
+      <c t="n" r="H6">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="n">
+      <c t="n" r="A7">
         <v>7698</v>
       </c>
-      <c r="B7" t="s">
+      <c t="s" r="B7">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c t="s" r="C7">
         <v>18</v>
       </c>
-      <c r="D7" t="n">
+      <c t="n" r="D7">
         <v>7839</v>
       </c>
-      <c r="E7" t="s">
+      <c t="s" r="E7">
         <v>23</v>
       </c>
-      <c r="F7" t="n">
+      <c t="n" r="F7">
         <v>2850</v>
       </c>
-      <c r="G7" t="s"/>
-      <c r="H7" t="n">
+      <c t="s" r="G7"/>
+      <c t="n" r="H7">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="n">
+      <c t="n" r="A8">
         <v>7782</v>
       </c>
-      <c r="B8" t="s">
+      <c t="s" r="B8">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c t="s" r="C8">
         <v>18</v>
       </c>
-      <c r="D8" t="n">
+      <c t="n" r="D8">
         <v>7839</v>
       </c>
-      <c r="E8" t="s">
+      <c t="s" r="E8">
         <v>25</v>
       </c>
-      <c r="F8" t="n">
+      <c t="n" r="F8">
         <v>2450</v>
       </c>
-      <c r="G8" t="s"/>
-      <c r="H8" t="n">
+      <c t="s" r="G8"/>
+      <c t="n" r="H8">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="n">
+      <c t="n" r="A9">
         <v>7788</v>
       </c>
-      <c r="B9" t="s">
+      <c t="s" r="B9">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c t="s" r="C9">
         <v>27</v>
       </c>
-      <c r="D9" t="n">
+      <c t="n" r="D9">
         <v>7566</v>
       </c>
-      <c r="E9" t="s">
+      <c t="s" r="E9">
         <v>28</v>
       </c>
-      <c r="F9" t="n">
+      <c t="n" r="F9">
         <v>3000</v>
       </c>
-      <c r="G9" t="s"/>
-      <c r="H9" t="n">
+      <c t="s" r="G9"/>
+      <c t="n" r="H9">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" t="n">
+      <c t="n" r="A10">
         <v>7839</v>
       </c>
-      <c r="B10" t="s">
+      <c t="s" r="B10">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c t="s" r="C10">
         <v>30</v>
       </c>
-      <c r="D10" t="s"/>
-      <c r="E10" t="s">
+      <c t="s" r="D10"/>
+      <c t="s" r="E10">
         <v>31</v>
       </c>
-      <c r="F10" t="n">
+      <c t="n" r="F10">
         <v>5000</v>
       </c>
-      <c r="G10" t="s"/>
-      <c r="H10" t="n">
+      <c t="s" r="G10"/>
+      <c t="n" r="H10">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" t="n">
+      <c t="n" r="A11">
         <v>7876</v>
       </c>
-      <c r="B11" t="s">
+      <c t="s" r="B11">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c t="s" r="C11">
         <v>33</v>
       </c>
-      <c r="D11" t="n">
+      <c t="n" r="D11">
         <v>7788</v>
       </c>
-      <c r="E11" t="s">
+      <c t="s" r="E11">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
+      <c t="s" r="F11">
         <v>35</v>
       </c>
-      <c r="G11" t="s"/>
-      <c r="H11" t="n">
+      <c t="s" r="G11"/>
+      <c t="n" r="H11">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" t="n">
+      <c t="n" r="A12">
         <v>7900</v>
       </c>
-      <c r="B12" t="s">
+      <c t="s" r="B12">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c t="s" r="C12">
         <v>33</v>
       </c>
-      <c r="D12" t="n">
+      <c t="n" r="D12">
         <v>7698</v>
       </c>
-      <c r="E12" t="s">
+      <c t="s" r="E12">
         <v>37</v>
       </c>
-      <c r="F12" t="n">
+      <c t="n" r="F12">
         <v>950</v>
       </c>
-      <c r="G12" t="s"/>
-      <c r="H12" t="n">
+      <c t="s" r="G12"/>
+      <c t="n" r="H12">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" t="n">
+      <c t="n" r="A13">
         <v>7902</v>
       </c>
-      <c r="B13" t="s">
+      <c t="s" r="B13">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c t="s" r="C13">
         <v>27</v>
       </c>
-      <c r="D13" t="n">
+      <c t="n" r="D13">
         <v>7566</v>
       </c>
-      <c r="E13" t="s">
+      <c t="s" r="E13">
         <v>37</v>
       </c>
-      <c r="F13" t="n">
+      <c t="n" r="F13">
         <v>3000</v>
       </c>
-      <c r="G13" t="s"/>
-      <c r="H13" t="n">
+      <c t="s" r="G13"/>
+      <c t="n" r="H13">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
QAL 0.4.0 (Linux changes)
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -494,320 +494,320 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c t="n" r="A2">
+      <c r="A2" t="n">
         <v>7369</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c t="n" r="D2">
+      <c r="D2" t="n">
         <v>7902</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c t="n" r="F2">
+      <c r="F2" t="n">
         <v>800</v>
       </c>
-      <c t="s" r="G2"/>
-      <c t="n" r="H2">
+      <c r="G2" t="s"/>
+      <c r="H2" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c t="n" r="A3">
+      <c r="A3" t="n">
         <v>7499</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="C3">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c t="n" r="D3">
+      <c r="D3" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E3">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c t="n" r="F3">
+      <c r="F3" t="n">
         <v>1600</v>
       </c>
-      <c t="n" r="G3">
+      <c r="G3" t="n">
         <v>300</v>
       </c>
-      <c t="n" r="H3">
+      <c r="H3" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c t="n" r="A4">
+      <c r="A4" t="n">
         <v>7521</v>
       </c>
-      <c t="s" r="B4">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c t="n" r="D4">
+      <c r="D4" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E4">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="F4">
+      <c r="F4" t="n">
         <v>1250</v>
       </c>
-      <c t="n" r="G4">
+      <c r="G4" t="n">
         <v>500</v>
       </c>
-      <c t="n" r="H4">
+      <c r="H4" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c t="n" r="A5">
+      <c r="A5" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D5">
+      <c r="D5" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E5">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c t="n" r="F5">
+      <c r="F5" t="n">
         <v>2975</v>
       </c>
-      <c t="s" r="G5"/>
-      <c t="n" r="H5">
+      <c r="G5" t="s"/>
+      <c r="H5" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c t="n" r="A6">
+      <c r="A6" t="n">
         <v>7654</v>
       </c>
-      <c t="s" r="B6">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="C6">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c t="n" r="D6">
+      <c r="D6" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E6">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c t="n" r="F6">
+      <c r="F6" t="n">
         <v>1250</v>
       </c>
-      <c t="n" r="G6">
+      <c r="G6" t="n">
         <v>1400</v>
       </c>
-      <c t="n" r="H6">
+      <c r="H6" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c t="n" r="A7">
+      <c r="A7" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D7">
+      <c r="D7" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E7">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c t="n" r="F7">
+      <c r="F7" t="n">
         <v>2850</v>
       </c>
-      <c t="s" r="G7"/>
-      <c t="n" r="H7">
+      <c r="G7" t="s"/>
+      <c r="H7" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c t="n" r="A8">
+      <c r="A8" t="n">
         <v>7782</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D8">
+      <c r="D8" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E8">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c t="n" r="F8">
+      <c r="F8" t="n">
         <v>2450</v>
       </c>
-      <c t="s" r="G8"/>
-      <c t="n" r="H8">
+      <c r="G8" t="s"/>
+      <c r="H8" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c t="n" r="A9">
+      <c r="A9" t="n">
         <v>7788</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c t="n" r="D9">
+      <c r="D9" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="E9">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c t="n" r="F9">
+      <c r="F9" t="n">
         <v>3000</v>
       </c>
-      <c t="s" r="G9"/>
-      <c t="n" r="H9">
+      <c r="G9" t="s"/>
+      <c r="H9" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c t="n" r="A10">
+      <c r="A10" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="D10"/>
-      <c t="s" r="E10">
+      <c r="D10" t="s"/>
+      <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c t="n" r="F10">
+      <c r="F10" t="n">
         <v>5000</v>
       </c>
-      <c t="s" r="G10"/>
-      <c t="n" r="H10">
+      <c r="G10" t="s"/>
+      <c r="H10" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c t="n" r="A11">
+      <c r="A11" t="n">
         <v>7876</v>
       </c>
-      <c t="s" r="B11">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c t="n" r="D11">
+      <c r="D11" t="n">
         <v>7788</v>
       </c>
-      <c t="s" r="E11">
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="F11">
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c t="s" r="G11"/>
-      <c t="n" r="H11">
+      <c r="G11" t="s"/>
+      <c r="H11" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c t="n" r="A12">
+      <c r="A12" t="n">
         <v>7900</v>
       </c>
-      <c t="s" r="B12">
+      <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c t="n" r="D12">
+      <c r="D12" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E12">
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c t="n" r="F12">
+      <c r="F12" t="n">
         <v>950</v>
       </c>
-      <c t="s" r="G12"/>
-      <c t="n" r="H12">
+      <c r="G12" t="s"/>
+      <c r="H12" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c t="n" r="A13">
+      <c r="A13" t="n">
         <v>7902</v>
       </c>
-      <c t="s" r="B13">
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="C13">
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c t="n" r="D13">
+      <c r="D13" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="E13">
+      <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c t="n" r="F13">
+      <c r="F13" t="n">
         <v>3000</v>
       </c>
-      <c t="s" r="G13"/>
-      <c t="n" r="H13">
+      <c r="G13" t="s"/>
+      <c r="H13" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve diff reporting Add support for the remaining datasets
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr/>
   <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" r:id="rId1"/>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </s:sheets>
   <s:definedNames/>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
 </s:workbook>
 </file>
 
@@ -142,16 +141,16 @@
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -465,9 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+  <s:sheetPr xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+    <s:pageSetUpPr/>
+  </s:sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -482,9 +482,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+  <s:sheetPr xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+    <s:pageSetUpPr/>
+  </s:sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Further typing for schemata
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -494,7 +494,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row spans="1:8" r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row spans="1:8" r="2">
       <c r="A2" t="n">
         <v>7369</v>
       </c>
@@ -544,7 +544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row spans="1:8" r="3">
       <c r="A3" t="n">
         <v>7499</v>
       </c>
@@ -570,7 +570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row spans="1:8" r="4">
       <c r="A4" t="n">
         <v>7521</v>
       </c>
@@ -596,7 +596,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row spans="1:8" r="5">
       <c r="A5" t="n">
         <v>7566</v>
       </c>
@@ -620,7 +620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row spans="1:8" r="6">
       <c r="A6" t="n">
         <v>7654</v>
       </c>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row spans="1:8" r="7">
       <c r="A7" t="n">
         <v>7698</v>
       </c>
@@ -670,7 +670,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row spans="1:8" r="8">
       <c r="A8" t="n">
         <v>7782</v>
       </c>
@@ -694,7 +694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row spans="1:8" r="9">
       <c r="A9" t="n">
         <v>7788</v>
       </c>
@@ -718,7 +718,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row spans="1:8" r="10">
       <c r="A10" t="n">
         <v>7839</v>
       </c>
@@ -740,7 +740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row spans="1:8" r="11">
       <c r="A11" t="n">
         <v>7876</v>
       </c>
@@ -764,7 +764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row spans="1:8" r="12">
       <c r="A12" t="n">
         <v>7900</v>
       </c>
@@ -788,7 +788,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row spans="1:8" r="13">
       <c r="A13" t="n">
         <v>7902</v>
       </c>

</xml_diff>

<commit_message>
Rename resource uuid, type and name Generalize and break out meta
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -494,7 +494,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row spans="1:8" r="1">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row spans="1:8" r="2">
+    <row r="2" spans="1:8">
       <c r="A2" t="n">
         <v>7369</v>
       </c>
@@ -544,7 +544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="3">
+    <row r="3" spans="1:8">
       <c r="A3" t="n">
         <v>7499</v>
       </c>
@@ -570,7 +570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="4">
+    <row r="4" spans="1:8">
       <c r="A4" t="n">
         <v>7521</v>
       </c>
@@ -596,7 +596,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="5">
+    <row r="5" spans="1:8">
       <c r="A5" t="n">
         <v>7566</v>
       </c>
@@ -620,7 +620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="6">
+    <row r="6" spans="1:8">
       <c r="A6" t="n">
         <v>7654</v>
       </c>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="7">
+    <row r="7" spans="1:8">
       <c r="A7" t="n">
         <v>7698</v>
       </c>
@@ -670,7 +670,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="8">
+    <row r="8" spans="1:8">
       <c r="A8" t="n">
         <v>7782</v>
       </c>
@@ -694,7 +694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row spans="1:8" r="9">
+    <row r="9" spans="1:8">
       <c r="A9" t="n">
         <v>7788</v>
       </c>
@@ -718,7 +718,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="10">
+    <row r="10" spans="1:8">
       <c r="A10" t="n">
         <v>7839</v>
       </c>
@@ -740,7 +740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row spans="1:8" r="11">
+    <row r="11" spans="1:8">
       <c r="A11" t="n">
         <v>7876</v>
       </c>
@@ -764,7 +764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="12">
+    <row r="12" spans="1:8">
       <c r="A12" t="n">
         <v>7900</v>
       </c>
@@ -788,7 +788,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="13">
+    <row r="13" spans="1:8">
       <c r="A13" t="n">
         <v>7902</v>
       </c>

</xml_diff>

<commit_message>
Move add child property to meta
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -494,321 +494,321 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
+    <row spans="1:8" r="1">
+      <c t="s" r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="n">
+    <row spans="1:8" r="2">
+      <c t="n" r="A2">
         <v>7369</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>9</v>
       </c>
-      <c r="D2" t="n">
+      <c t="n" r="D2">
         <v>7902</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>10</v>
       </c>
-      <c r="F2" t="n">
+      <c t="n" r="F2">
         <v>800</v>
       </c>
-      <c r="G2" t="s"/>
-      <c r="H2" t="n">
+      <c t="s" r="G2"/>
+      <c t="n" r="H2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="n">
+    <row spans="1:8" r="3">
+      <c t="n" r="A3">
         <v>7499</v>
       </c>
-      <c r="B3" t="s">
+      <c t="s" r="B3">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c t="s" r="C3">
         <v>12</v>
       </c>
-      <c r="D3" t="n">
+      <c t="n" r="D3">
         <v>7698</v>
       </c>
-      <c r="E3" t="s">
+      <c t="s" r="E3">
         <v>13</v>
       </c>
-      <c r="F3" t="n">
+      <c t="n" r="F3">
         <v>1600</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>300</v>
       </c>
-      <c r="H3" t="n">
+      <c t="n" r="H3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="n">
+    <row spans="1:8" r="4">
+      <c t="n" r="A4">
         <v>7521</v>
       </c>
-      <c r="B4" t="s">
+      <c t="s" r="B4">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c t="s" r="C4">
         <v>15</v>
       </c>
-      <c r="D4" t="n">
+      <c t="n" r="D4">
         <v>7698</v>
       </c>
-      <c r="E4" t="s">
+      <c t="s" r="E4">
         <v>16</v>
       </c>
-      <c r="F4" t="n">
+      <c t="n" r="F4">
         <v>1250</v>
       </c>
-      <c r="G4" t="n">
+      <c t="n" r="G4">
         <v>500</v>
       </c>
-      <c r="H4" t="n">
+      <c t="n" r="H4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="n">
+    <row spans="1:8" r="5">
+      <c t="n" r="A5">
         <v>7566</v>
       </c>
-      <c r="B5" t="s">
+      <c t="s" r="B5">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c t="s" r="C5">
         <v>18</v>
       </c>
-      <c r="D5" t="n">
+      <c t="n" r="D5">
         <v>7839</v>
       </c>
-      <c r="E5" t="s">
+      <c t="s" r="E5">
         <v>19</v>
       </c>
-      <c r="F5" t="n">
+      <c t="n" r="F5">
         <v>2975</v>
       </c>
-      <c r="G5" t="s"/>
-      <c r="H5" t="n">
+      <c t="s" r="G5"/>
+      <c t="n" r="H5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="n">
+    <row spans="1:8" r="6">
+      <c t="n" r="A6">
         <v>7654</v>
       </c>
-      <c r="B6" t="s">
+      <c t="s" r="B6">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c t="s" r="C6">
         <v>15</v>
       </c>
-      <c r="D6" t="n">
+      <c t="n" r="D6">
         <v>7698</v>
       </c>
-      <c r="E6" t="s">
+      <c t="s" r="E6">
         <v>21</v>
       </c>
-      <c r="F6" t="n">
+      <c t="n" r="F6">
         <v>1250</v>
       </c>
-      <c r="G6" t="n">
+      <c t="n" r="G6">
         <v>1400</v>
       </c>
-      <c r="H6" t="n">
+      <c t="n" r="H6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="n">
+    <row spans="1:8" r="7">
+      <c t="n" r="A7">
         <v>7698</v>
       </c>
-      <c r="B7" t="s">
+      <c t="s" r="B7">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c t="s" r="C7">
         <v>18</v>
       </c>
-      <c r="D7" t="n">
+      <c t="n" r="D7">
         <v>7839</v>
       </c>
-      <c r="E7" t="s">
+      <c t="s" r="E7">
         <v>23</v>
       </c>
-      <c r="F7" t="n">
+      <c t="n" r="F7">
         <v>2850</v>
       </c>
-      <c r="G7" t="s"/>
-      <c r="H7" t="n">
+      <c t="s" r="G7"/>
+      <c t="n" r="H7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="n">
+    <row spans="1:8" r="8">
+      <c t="n" r="A8">
         <v>7782</v>
       </c>
-      <c r="B8" t="s">
+      <c t="s" r="B8">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c t="s" r="C8">
         <v>18</v>
       </c>
-      <c r="D8" t="n">
+      <c t="n" r="D8">
         <v>7839</v>
       </c>
-      <c r="E8" t="s">
+      <c t="s" r="E8">
         <v>25</v>
       </c>
-      <c r="F8" t="n">
+      <c t="n" r="F8">
         <v>2450</v>
       </c>
-      <c r="G8" t="s"/>
-      <c r="H8" t="n">
+      <c t="s" r="G8"/>
+      <c t="n" r="H8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="n">
+    <row spans="1:8" r="9">
+      <c t="n" r="A9">
         <v>7788</v>
       </c>
-      <c r="B9" t="s">
+      <c t="s" r="B9">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c t="s" r="C9">
         <v>27</v>
       </c>
-      <c r="D9" t="n">
+      <c t="n" r="D9">
         <v>7566</v>
       </c>
-      <c r="E9" t="s">
+      <c t="s" r="E9">
         <v>28</v>
       </c>
-      <c r="F9" t="n">
+      <c t="n" r="F9">
         <v>3000</v>
       </c>
-      <c r="G9" t="s"/>
-      <c r="H9" t="n">
+      <c t="s" r="G9"/>
+      <c t="n" r="H9">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="n">
+    <row spans="1:8" r="10">
+      <c t="n" r="A10">
         <v>7839</v>
       </c>
-      <c r="B10" t="s">
+      <c t="s" r="B10">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c t="s" r="C10">
         <v>30</v>
       </c>
-      <c r="D10" t="s"/>
-      <c r="E10" t="s">
+      <c t="s" r="D10"/>
+      <c t="s" r="E10">
         <v>31</v>
       </c>
-      <c r="F10" t="n">
+      <c t="n" r="F10">
         <v>5000</v>
       </c>
-      <c r="G10" t="s"/>
-      <c r="H10" t="n">
+      <c t="s" r="G10"/>
+      <c t="n" r="H10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="n">
+    <row spans="1:8" r="11">
+      <c t="n" r="A11">
         <v>7876</v>
       </c>
-      <c r="B11" t="s">
+      <c t="s" r="B11">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c t="s" r="C11">
         <v>33</v>
       </c>
-      <c r="D11" t="n">
+      <c t="n" r="D11">
         <v>7788</v>
       </c>
-      <c r="E11" t="s">
+      <c t="s" r="E11">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
+      <c t="s" r="F11">
         <v>35</v>
       </c>
-      <c r="G11" t="s"/>
-      <c r="H11" t="n">
+      <c t="s" r="G11"/>
+      <c t="n" r="H11">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="n">
+    <row spans="1:8" r="12">
+      <c t="n" r="A12">
         <v>7900</v>
       </c>
-      <c r="B12" t="s">
+      <c t="s" r="B12">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c t="s" r="C12">
         <v>33</v>
       </c>
-      <c r="D12" t="n">
+      <c t="n" r="D12">
         <v>7698</v>
       </c>
-      <c r="E12" t="s">
+      <c t="s" r="E12">
         <v>37</v>
       </c>
-      <c r="F12" t="n">
+      <c t="n" r="F12">
         <v>950</v>
       </c>
-      <c r="G12" t="s"/>
-      <c r="H12" t="n">
+      <c t="s" r="G12"/>
+      <c t="n" r="H12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="n">
+    <row spans="1:8" r="13">
+      <c t="n" r="A13">
         <v>7902</v>
       </c>
-      <c r="B13" t="s">
+      <c t="s" r="B13">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c t="s" r="C13">
         <v>27</v>
       </c>
-      <c r="D13" t="n">
+      <c t="n" r="D13">
         <v>7566</v>
       </c>
-      <c r="E13" t="s">
+      <c t="s" r="E13">
         <v>37</v>
       </c>
-      <c r="F13" t="n">
+      <c t="n" r="F13">
         <v>3000</v>
       </c>
-      <c r="G13" t="s"/>
-      <c r="H13" t="n">
+      <c t="s" r="G13"/>
+      <c t="n" r="H13">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create Recurse class Continue Resource(s) schema Move tools into common
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -494,7 +494,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row spans="1:8" r="1">
+    <row r="1" spans="1:8">
       <c t="s" r="A1">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row spans="1:8" r="2">
+    <row r="2" spans="1:8">
       <c t="n" r="A2">
         <v>7369</v>
       </c>
@@ -544,7 +544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="3">
+    <row r="3" spans="1:8">
       <c t="n" r="A3">
         <v>7499</v>
       </c>
@@ -570,7 +570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="4">
+    <row r="4" spans="1:8">
       <c t="n" r="A4">
         <v>7521</v>
       </c>
@@ -596,7 +596,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="5">
+    <row r="5" spans="1:8">
       <c t="n" r="A5">
         <v>7566</v>
       </c>
@@ -620,7 +620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="6">
+    <row r="6" spans="1:8">
       <c t="n" r="A6">
         <v>7654</v>
       </c>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="7">
+    <row r="7" spans="1:8">
       <c t="n" r="A7">
         <v>7698</v>
       </c>
@@ -670,7 +670,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="8">
+    <row r="8" spans="1:8">
       <c t="n" r="A8">
         <v>7782</v>
       </c>
@@ -694,7 +694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row spans="1:8" r="9">
+    <row r="9" spans="1:8">
       <c t="n" r="A9">
         <v>7788</v>
       </c>
@@ -718,7 +718,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="10">
+    <row r="10" spans="1:8">
       <c t="n" r="A10">
         <v>7839</v>
       </c>
@@ -740,7 +740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row spans="1:8" r="11">
+    <row r="11" spans="1:8">
       <c t="n" r="A11">
         <v>7876</v>
       </c>
@@ -764,7 +764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="12">
+    <row r="12" spans="1:8">
       <c t="n" r="A12">
         <v>7900</v>
       </c>
@@ -788,7 +788,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="13">
+    <row r="13" spans="1:8">
       <c t="n" r="A13">
         <v>7902</v>
       </c>

</xml_diff>

<commit_message>
Finalize merge to json to merge Improve resource validation
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -495,320 +495,320 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>7369</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>9</v>
       </c>
-      <c r="D2" t="n">
+      <c t="n" r="D2">
         <v>7902</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>10</v>
       </c>
-      <c r="F2" t="n">
+      <c t="n" r="F2">
         <v>800</v>
       </c>
-      <c r="G2" t="s"/>
-      <c r="H2" t="n">
+      <c t="s" r="G2"/>
+      <c t="n" r="H2">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="n">
+      <c t="n" r="A3">
         <v>7499</v>
       </c>
-      <c r="B3" t="s">
+      <c t="s" r="B3">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c t="s" r="C3">
         <v>12</v>
       </c>
-      <c r="D3" t="n">
+      <c t="n" r="D3">
         <v>7698</v>
       </c>
-      <c r="E3" t="s">
+      <c t="s" r="E3">
         <v>13</v>
       </c>
-      <c r="F3" t="n">
+      <c t="n" r="F3">
         <v>1600</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>300</v>
       </c>
-      <c r="H3" t="n">
+      <c t="n" r="H3">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="n">
+      <c t="n" r="A4">
         <v>7521</v>
       </c>
-      <c r="B4" t="s">
+      <c t="s" r="B4">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c t="s" r="C4">
         <v>15</v>
       </c>
-      <c r="D4" t="n">
+      <c t="n" r="D4">
         <v>7698</v>
       </c>
-      <c r="E4" t="s">
+      <c t="s" r="E4">
         <v>16</v>
       </c>
-      <c r="F4" t="n">
+      <c t="n" r="F4">
         <v>1250</v>
       </c>
-      <c r="G4" t="n">
+      <c t="n" r="G4">
         <v>500</v>
       </c>
-      <c r="H4" t="n">
+      <c t="n" r="H4">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="n">
+      <c t="n" r="A5">
         <v>7566</v>
       </c>
-      <c r="B5" t="s">
+      <c t="s" r="B5">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c t="s" r="C5">
         <v>18</v>
       </c>
-      <c r="D5" t="n">
+      <c t="n" r="D5">
         <v>7839</v>
       </c>
-      <c r="E5" t="s">
+      <c t="s" r="E5">
         <v>19</v>
       </c>
-      <c r="F5" t="n">
+      <c t="n" r="F5">
         <v>2975</v>
       </c>
-      <c r="G5" t="s"/>
-      <c r="H5" t="n">
+      <c t="s" r="G5"/>
+      <c t="n" r="H5">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="n">
+      <c t="n" r="A6">
         <v>7654</v>
       </c>
-      <c r="B6" t="s">
+      <c t="s" r="B6">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c t="s" r="C6">
         <v>15</v>
       </c>
-      <c r="D6" t="n">
+      <c t="n" r="D6">
         <v>7698</v>
       </c>
-      <c r="E6" t="s">
+      <c t="s" r="E6">
         <v>21</v>
       </c>
-      <c r="F6" t="n">
+      <c t="n" r="F6">
         <v>1250</v>
       </c>
-      <c r="G6" t="n">
+      <c t="n" r="G6">
         <v>1400</v>
       </c>
-      <c r="H6" t="n">
+      <c t="n" r="H6">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="n">
+      <c t="n" r="A7">
         <v>7698</v>
       </c>
-      <c r="B7" t="s">
+      <c t="s" r="B7">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c t="s" r="C7">
         <v>18</v>
       </c>
-      <c r="D7" t="n">
+      <c t="n" r="D7">
         <v>7839</v>
       </c>
-      <c r="E7" t="s">
+      <c t="s" r="E7">
         <v>23</v>
       </c>
-      <c r="F7" t="n">
+      <c t="n" r="F7">
         <v>2850</v>
       </c>
-      <c r="G7" t="s"/>
-      <c r="H7" t="n">
+      <c t="s" r="G7"/>
+      <c t="n" r="H7">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="n">
+      <c t="n" r="A8">
         <v>7782</v>
       </c>
-      <c r="B8" t="s">
+      <c t="s" r="B8">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c t="s" r="C8">
         <v>18</v>
       </c>
-      <c r="D8" t="n">
+      <c t="n" r="D8">
         <v>7839</v>
       </c>
-      <c r="E8" t="s">
+      <c t="s" r="E8">
         <v>25</v>
       </c>
-      <c r="F8" t="n">
+      <c t="n" r="F8">
         <v>2450</v>
       </c>
-      <c r="G8" t="s"/>
-      <c r="H8" t="n">
+      <c t="s" r="G8"/>
+      <c t="n" r="H8">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="n">
+      <c t="n" r="A9">
         <v>7788</v>
       </c>
-      <c r="B9" t="s">
+      <c t="s" r="B9">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c t="s" r="C9">
         <v>27</v>
       </c>
-      <c r="D9" t="n">
+      <c t="n" r="D9">
         <v>7566</v>
       </c>
-      <c r="E9" t="s">
+      <c t="s" r="E9">
         <v>28</v>
       </c>
-      <c r="F9" t="n">
+      <c t="n" r="F9">
         <v>3000</v>
       </c>
-      <c r="G9" t="s"/>
-      <c r="H9" t="n">
+      <c t="s" r="G9"/>
+      <c t="n" r="H9">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" t="n">
+      <c t="n" r="A10">
         <v>7839</v>
       </c>
-      <c r="B10" t="s">
+      <c t="s" r="B10">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c t="s" r="C10">
         <v>30</v>
       </c>
-      <c r="D10" t="s"/>
-      <c r="E10" t="s">
+      <c t="s" r="D10"/>
+      <c t="s" r="E10">
         <v>31</v>
       </c>
-      <c r="F10" t="n">
+      <c t="n" r="F10">
         <v>5000</v>
       </c>
-      <c r="G10" t="s"/>
-      <c r="H10" t="n">
+      <c t="s" r="G10"/>
+      <c t="n" r="H10">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" t="n">
+      <c t="n" r="A11">
         <v>7876</v>
       </c>
-      <c r="B11" t="s">
+      <c t="s" r="B11">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c t="s" r="C11">
         <v>33</v>
       </c>
-      <c r="D11" t="n">
+      <c t="n" r="D11">
         <v>7788</v>
       </c>
-      <c r="E11" t="s">
+      <c t="s" r="E11">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
+      <c t="s" r="F11">
         <v>35</v>
       </c>
-      <c r="G11" t="s"/>
-      <c r="H11" t="n">
+      <c t="s" r="G11"/>
+      <c t="n" r="H11">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" t="n">
+      <c t="n" r="A12">
         <v>7900</v>
       </c>
-      <c r="B12" t="s">
+      <c t="s" r="B12">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c t="s" r="C12">
         <v>33</v>
       </c>
-      <c r="D12" t="n">
+      <c t="n" r="D12">
         <v>7698</v>
       </c>
-      <c r="E12" t="s">
+      <c t="s" r="E12">
         <v>37</v>
       </c>
-      <c r="F12" t="n">
+      <c t="n" r="F12">
         <v>950</v>
       </c>
-      <c r="G12" t="s"/>
-      <c r="H12" t="n">
+      <c t="s" r="G12"/>
+      <c t="n" r="H12">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" t="n">
+      <c t="n" r="A13">
         <v>7902</v>
       </c>
-      <c r="B13" t="s">
+      <c t="s" r="B13">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c t="s" r="C13">
         <v>27</v>
       </c>
-      <c r="D13" t="n">
+      <c t="n" r="D13">
         <v>7566</v>
       </c>
-      <c r="E13" t="s">
+      <c t="s" r="E13">
         <v>37</v>
       </c>
-      <c r="F13" t="n">
+      <c t="n" r="F13">
         <v>3000</v>
       </c>
-      <c r="G13" t="s"/>
-      <c r="H13" t="n">
+      <c t="s" r="G13"/>
+      <c t="n" r="H13">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix residual problem with SQL-json
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -494,321 +494,321 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
+    <row spans="1:8" r="1">
+      <c t="s" r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="n">
+    <row spans="1:8" r="2">
+      <c t="n" r="A2">
         <v>7369</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>9</v>
       </c>
-      <c r="D2" t="n">
+      <c t="n" r="D2">
         <v>7902</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>10</v>
       </c>
-      <c r="F2" t="n">
+      <c t="n" r="F2">
         <v>800</v>
       </c>
-      <c r="G2" t="s"/>
-      <c r="H2" t="n">
+      <c t="s" r="G2"/>
+      <c t="n" r="H2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="n">
+    <row spans="1:8" r="3">
+      <c t="n" r="A3">
         <v>7499</v>
       </c>
-      <c r="B3" t="s">
+      <c t="s" r="B3">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c t="s" r="C3">
         <v>12</v>
       </c>
-      <c r="D3" t="n">
+      <c t="n" r="D3">
         <v>7698</v>
       </c>
-      <c r="E3" t="s">
+      <c t="s" r="E3">
         <v>13</v>
       </c>
-      <c r="F3" t="n">
+      <c t="n" r="F3">
         <v>1600</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>300</v>
       </c>
-      <c r="H3" t="n">
+      <c t="n" r="H3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="n">
+    <row spans="1:8" r="4">
+      <c t="n" r="A4">
         <v>7521</v>
       </c>
-      <c r="B4" t="s">
+      <c t="s" r="B4">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c t="s" r="C4">
         <v>15</v>
       </c>
-      <c r="D4" t="n">
+      <c t="n" r="D4">
         <v>7698</v>
       </c>
-      <c r="E4" t="s">
+      <c t="s" r="E4">
         <v>16</v>
       </c>
-      <c r="F4" t="n">
+      <c t="n" r="F4">
         <v>1250</v>
       </c>
-      <c r="G4" t="n">
+      <c t="n" r="G4">
         <v>500</v>
       </c>
-      <c r="H4" t="n">
+      <c t="n" r="H4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="n">
+    <row spans="1:8" r="5">
+      <c t="n" r="A5">
         <v>7566</v>
       </c>
-      <c r="B5" t="s">
+      <c t="s" r="B5">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c t="s" r="C5">
         <v>18</v>
       </c>
-      <c r="D5" t="n">
+      <c t="n" r="D5">
         <v>7839</v>
       </c>
-      <c r="E5" t="s">
+      <c t="s" r="E5">
         <v>19</v>
       </c>
-      <c r="F5" t="n">
+      <c t="n" r="F5">
         <v>2975</v>
       </c>
-      <c r="G5" t="s"/>
-      <c r="H5" t="n">
+      <c t="s" r="G5"/>
+      <c t="n" r="H5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="n">
+    <row spans="1:8" r="6">
+      <c t="n" r="A6">
         <v>7654</v>
       </c>
-      <c r="B6" t="s">
+      <c t="s" r="B6">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c t="s" r="C6">
         <v>15</v>
       </c>
-      <c r="D6" t="n">
+      <c t="n" r="D6">
         <v>7698</v>
       </c>
-      <c r="E6" t="s">
+      <c t="s" r="E6">
         <v>21</v>
       </c>
-      <c r="F6" t="n">
+      <c t="n" r="F6">
         <v>1250</v>
       </c>
-      <c r="G6" t="n">
+      <c t="n" r="G6">
         <v>1400</v>
       </c>
-      <c r="H6" t="n">
+      <c t="n" r="H6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="n">
+    <row spans="1:8" r="7">
+      <c t="n" r="A7">
         <v>7698</v>
       </c>
-      <c r="B7" t="s">
+      <c t="s" r="B7">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c t="s" r="C7">
         <v>18</v>
       </c>
-      <c r="D7" t="n">
+      <c t="n" r="D7">
         <v>7839</v>
       </c>
-      <c r="E7" t="s">
+      <c t="s" r="E7">
         <v>23</v>
       </c>
-      <c r="F7" t="n">
+      <c t="n" r="F7">
         <v>2850</v>
       </c>
-      <c r="G7" t="s"/>
-      <c r="H7" t="n">
+      <c t="s" r="G7"/>
+      <c t="n" r="H7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="n">
+    <row spans="1:8" r="8">
+      <c t="n" r="A8">
         <v>7782</v>
       </c>
-      <c r="B8" t="s">
+      <c t="s" r="B8">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c t="s" r="C8">
         <v>18</v>
       </c>
-      <c r="D8" t="n">
+      <c t="n" r="D8">
         <v>7839</v>
       </c>
-      <c r="E8" t="s">
+      <c t="s" r="E8">
         <v>25</v>
       </c>
-      <c r="F8" t="n">
+      <c t="n" r="F8">
         <v>2450</v>
       </c>
-      <c r="G8" t="s"/>
-      <c r="H8" t="n">
+      <c t="s" r="G8"/>
+      <c t="n" r="H8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="n">
+    <row spans="1:8" r="9">
+      <c t="n" r="A9">
         <v>7788</v>
       </c>
-      <c r="B9" t="s">
+      <c t="s" r="B9">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c t="s" r="C9">
         <v>27</v>
       </c>
-      <c r="D9" t="n">
+      <c t="n" r="D9">
         <v>7566</v>
       </c>
-      <c r="E9" t="s">
+      <c t="s" r="E9">
         <v>28</v>
       </c>
-      <c r="F9" t="n">
+      <c t="n" r="F9">
         <v>3000</v>
       </c>
-      <c r="G9" t="s"/>
-      <c r="H9" t="n">
+      <c t="s" r="G9"/>
+      <c t="n" r="H9">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="n">
+    <row spans="1:8" r="10">
+      <c t="n" r="A10">
         <v>7839</v>
       </c>
-      <c r="B10" t="s">
+      <c t="s" r="B10">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c t="s" r="C10">
         <v>30</v>
       </c>
-      <c r="D10" t="s"/>
-      <c r="E10" t="s">
+      <c t="s" r="D10"/>
+      <c t="s" r="E10">
         <v>31</v>
       </c>
-      <c r="F10" t="n">
+      <c t="n" r="F10">
         <v>5000</v>
       </c>
-      <c r="G10" t="s"/>
-      <c r="H10" t="n">
+      <c t="s" r="G10"/>
+      <c t="n" r="H10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="n">
+    <row spans="1:8" r="11">
+      <c t="n" r="A11">
         <v>7876</v>
       </c>
-      <c r="B11" t="s">
+      <c t="s" r="B11">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c t="s" r="C11">
         <v>33</v>
       </c>
-      <c r="D11" t="n">
+      <c t="n" r="D11">
         <v>7788</v>
       </c>
-      <c r="E11" t="s">
+      <c t="s" r="E11">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
+      <c t="s" r="F11">
         <v>35</v>
       </c>
-      <c r="G11" t="s"/>
-      <c r="H11" t="n">
+      <c t="s" r="G11"/>
+      <c t="n" r="H11">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="n">
+    <row spans="1:8" r="12">
+      <c t="n" r="A12">
         <v>7900</v>
       </c>
-      <c r="B12" t="s">
+      <c t="s" r="B12">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c t="s" r="C12">
         <v>33</v>
       </c>
-      <c r="D12" t="n">
+      <c t="n" r="D12">
         <v>7698</v>
       </c>
-      <c r="E12" t="s">
+      <c t="s" r="E12">
         <v>37</v>
       </c>
-      <c r="F12" t="n">
+      <c t="n" r="F12">
         <v>950</v>
       </c>
-      <c r="G12" t="s"/>
-      <c r="H12" t="n">
+      <c t="s" r="G12"/>
+      <c t="n" r="H12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="n">
+    <row spans="1:8" r="13">
+      <c t="n" r="A13">
         <v>7902</v>
       </c>
-      <c r="B13" t="s">
+      <c t="s" r="B13">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c t="s" r="C13">
         <v>27</v>
       </c>
-      <c r="D13" t="n">
+      <c t="n" r="D13">
         <v>7566</v>
       </c>
-      <c r="E13" t="s">
+      <c t="s" r="E13">
         <v>37</v>
       </c>
-      <c r="F13" t="n">
+      <c t="n" r="F13">
         <v>3000</v>
       </c>
-      <c r="G13" t="s"/>
-      <c r="H13" t="n">
+      <c t="s" r="G13"/>
+      <c t="n" r="H13">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix json-schema resolution by adding a referrer Add datasets to json-schema
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -494,321 +494,321 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row spans="1:8" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row spans="1:8" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:8">
+      <c r="A2" t="n">
         <v>7369</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c t="n" r="D2">
+      <c r="D2" t="n">
         <v>7902</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c t="n" r="F2">
+      <c r="F2" t="n">
         <v>800</v>
       </c>
-      <c t="s" r="G2"/>
-      <c t="n" r="H2">
+      <c r="G2" t="s"/>
+      <c r="H2" t="n">
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:8">
+      <c r="A3" t="n">
         <v>7499</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="C3">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c t="n" r="D3">
+      <c r="D3" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E3">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c t="n" r="F3">
+      <c r="F3" t="n">
         <v>1600</v>
       </c>
-      <c t="n" r="G3">
+      <c r="G3" t="n">
         <v>300</v>
       </c>
-      <c t="n" r="H3">
+      <c r="H3" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="4">
-      <c t="n" r="A4">
+    <row r="4" spans="1:8">
+      <c r="A4" t="n">
         <v>7521</v>
       </c>
-      <c t="s" r="B4">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c t="n" r="D4">
+      <c r="D4" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E4">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="F4">
+      <c r="F4" t="n">
         <v>1250</v>
       </c>
-      <c t="n" r="G4">
+      <c r="G4" t="n">
         <v>500</v>
       </c>
-      <c t="n" r="H4">
+      <c r="H4" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="5">
-      <c t="n" r="A5">
+    <row r="5" spans="1:8">
+      <c r="A5" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D5">
+      <c r="D5" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E5">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c t="n" r="F5">
+      <c r="F5" t="n">
         <v>2975</v>
       </c>
-      <c t="s" r="G5"/>
-      <c t="n" r="H5">
+      <c r="G5" t="s"/>
+      <c r="H5" t="n">
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="6">
-      <c t="n" r="A6">
+    <row r="6" spans="1:8">
+      <c r="A6" t="n">
         <v>7654</v>
       </c>
-      <c t="s" r="B6">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="C6">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c t="n" r="D6">
+      <c r="D6" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E6">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c t="n" r="F6">
+      <c r="F6" t="n">
         <v>1250</v>
       </c>
-      <c t="n" r="G6">
+      <c r="G6" t="n">
         <v>1400</v>
       </c>
-      <c t="n" r="H6">
+      <c r="H6" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="7">
-      <c t="n" r="A7">
+    <row r="7" spans="1:8">
+      <c r="A7" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D7">
+      <c r="D7" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E7">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c t="n" r="F7">
+      <c r="F7" t="n">
         <v>2850</v>
       </c>
-      <c t="s" r="G7"/>
-      <c t="n" r="H7">
+      <c r="G7" t="s"/>
+      <c r="H7" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="8">
-      <c t="n" r="A8">
+    <row r="8" spans="1:8">
+      <c r="A8" t="n">
         <v>7782</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D8">
+      <c r="D8" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E8">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c t="n" r="F8">
+      <c r="F8" t="n">
         <v>2450</v>
       </c>
-      <c t="s" r="G8"/>
-      <c t="n" r="H8">
+      <c r="G8" t="s"/>
+      <c r="H8" t="n">
         <v>10</v>
       </c>
     </row>
-    <row spans="1:8" r="9">
-      <c t="n" r="A9">
+    <row r="9" spans="1:8">
+      <c r="A9" t="n">
         <v>7788</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c t="n" r="D9">
+      <c r="D9" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="E9">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c t="n" r="F9">
+      <c r="F9" t="n">
         <v>3000</v>
       </c>
-      <c t="s" r="G9"/>
-      <c t="n" r="H9">
+      <c r="G9" t="s"/>
+      <c r="H9" t="n">
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="10">
-      <c t="n" r="A10">
+    <row r="10" spans="1:8">
+      <c r="A10" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="D10"/>
-      <c t="s" r="E10">
+      <c r="D10" t="s"/>
+      <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c t="n" r="F10">
+      <c r="F10" t="n">
         <v>5000</v>
       </c>
-      <c t="s" r="G10"/>
-      <c t="n" r="H10">
+      <c r="G10" t="s"/>
+      <c r="H10" t="n">
         <v>10</v>
       </c>
     </row>
-    <row spans="1:8" r="11">
-      <c t="n" r="A11">
+    <row r="11" spans="1:8">
+      <c r="A11" t="n">
         <v>7876</v>
       </c>
-      <c t="s" r="B11">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c t="n" r="D11">
+      <c r="D11" t="n">
         <v>7788</v>
       </c>
-      <c t="s" r="E11">
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="F11">
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c t="s" r="G11"/>
-      <c t="n" r="H11">
+      <c r="G11" t="s"/>
+      <c r="H11" t="n">
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="12">
-      <c t="n" r="A12">
+    <row r="12" spans="1:8">
+      <c r="A12" t="n">
         <v>7900</v>
       </c>
-      <c t="s" r="B12">
+      <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c t="n" r="D12">
+      <c r="D12" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E12">
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c t="n" r="F12">
+      <c r="F12" t="n">
         <v>950</v>
       </c>
-      <c t="s" r="G12"/>
-      <c t="n" r="H12">
+      <c r="G12" t="s"/>
+      <c r="H12" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="13">
-      <c t="n" r="A13">
+    <row r="13" spans="1:8">
+      <c r="A13" t="n">
         <v>7902</v>
       </c>
-      <c t="s" r="B13">
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="C13">
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c t="n" r="D13">
+      <c r="D13" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="E13">
+      <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c t="n" r="F13">
+      <c r="F13" t="n">
         <v>3000</v>
       </c>
-      <c t="s" r="G13"/>
-      <c t="n" r="H13">
+      <c r="G13" t="s"/>
+      <c r="H13" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve the scheme resolution
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -495,320 +495,320 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>7369</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>9</v>
       </c>
-      <c r="D2" t="n">
+      <c t="n" r="D2">
         <v>7902</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>10</v>
       </c>
-      <c r="F2" t="n">
+      <c t="n" r="F2">
         <v>800</v>
       </c>
-      <c r="G2" t="s"/>
-      <c r="H2" t="n">
+      <c t="s" r="G2"/>
+      <c t="n" r="H2">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="n">
+      <c t="n" r="A3">
         <v>7499</v>
       </c>
-      <c r="B3" t="s">
+      <c t="s" r="B3">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c t="s" r="C3">
         <v>12</v>
       </c>
-      <c r="D3" t="n">
+      <c t="n" r="D3">
         <v>7698</v>
       </c>
-      <c r="E3" t="s">
+      <c t="s" r="E3">
         <v>13</v>
       </c>
-      <c r="F3" t="n">
+      <c t="n" r="F3">
         <v>1600</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>300</v>
       </c>
-      <c r="H3" t="n">
+      <c t="n" r="H3">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="n">
+      <c t="n" r="A4">
         <v>7521</v>
       </c>
-      <c r="B4" t="s">
+      <c t="s" r="B4">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c t="s" r="C4">
         <v>15</v>
       </c>
-      <c r="D4" t="n">
+      <c t="n" r="D4">
         <v>7698</v>
       </c>
-      <c r="E4" t="s">
+      <c t="s" r="E4">
         <v>16</v>
       </c>
-      <c r="F4" t="n">
+      <c t="n" r="F4">
         <v>1250</v>
       </c>
-      <c r="G4" t="n">
+      <c t="n" r="G4">
         <v>500</v>
       </c>
-      <c r="H4" t="n">
+      <c t="n" r="H4">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="n">
+      <c t="n" r="A5">
         <v>7566</v>
       </c>
-      <c r="B5" t="s">
+      <c t="s" r="B5">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c t="s" r="C5">
         <v>18</v>
       </c>
-      <c r="D5" t="n">
+      <c t="n" r="D5">
         <v>7839</v>
       </c>
-      <c r="E5" t="s">
+      <c t="s" r="E5">
         <v>19</v>
       </c>
-      <c r="F5" t="n">
+      <c t="n" r="F5">
         <v>2975</v>
       </c>
-      <c r="G5" t="s"/>
-      <c r="H5" t="n">
+      <c t="s" r="G5"/>
+      <c t="n" r="H5">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="n">
+      <c t="n" r="A6">
         <v>7654</v>
       </c>
-      <c r="B6" t="s">
+      <c t="s" r="B6">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c t="s" r="C6">
         <v>15</v>
       </c>
-      <c r="D6" t="n">
+      <c t="n" r="D6">
         <v>7698</v>
       </c>
-      <c r="E6" t="s">
+      <c t="s" r="E6">
         <v>21</v>
       </c>
-      <c r="F6" t="n">
+      <c t="n" r="F6">
         <v>1250</v>
       </c>
-      <c r="G6" t="n">
+      <c t="n" r="G6">
         <v>1400</v>
       </c>
-      <c r="H6" t="n">
+      <c t="n" r="H6">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="n">
+      <c t="n" r="A7">
         <v>7698</v>
       </c>
-      <c r="B7" t="s">
+      <c t="s" r="B7">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c t="s" r="C7">
         <v>18</v>
       </c>
-      <c r="D7" t="n">
+      <c t="n" r="D7">
         <v>7839</v>
       </c>
-      <c r="E7" t="s">
+      <c t="s" r="E7">
         <v>23</v>
       </c>
-      <c r="F7" t="n">
+      <c t="n" r="F7">
         <v>2850</v>
       </c>
-      <c r="G7" t="s"/>
-      <c r="H7" t="n">
+      <c t="s" r="G7"/>
+      <c t="n" r="H7">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="n">
+      <c t="n" r="A8">
         <v>7782</v>
       </c>
-      <c r="B8" t="s">
+      <c t="s" r="B8">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c t="s" r="C8">
         <v>18</v>
       </c>
-      <c r="D8" t="n">
+      <c t="n" r="D8">
         <v>7839</v>
       </c>
-      <c r="E8" t="s">
+      <c t="s" r="E8">
         <v>25</v>
       </c>
-      <c r="F8" t="n">
+      <c t="n" r="F8">
         <v>2450</v>
       </c>
-      <c r="G8" t="s"/>
-      <c r="H8" t="n">
+      <c t="s" r="G8"/>
+      <c t="n" r="H8">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="n">
+      <c t="n" r="A9">
         <v>7788</v>
       </c>
-      <c r="B9" t="s">
+      <c t="s" r="B9">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c t="s" r="C9">
         <v>27</v>
       </c>
-      <c r="D9" t="n">
+      <c t="n" r="D9">
         <v>7566</v>
       </c>
-      <c r="E9" t="s">
+      <c t="s" r="E9">
         <v>28</v>
       </c>
-      <c r="F9" t="n">
+      <c t="n" r="F9">
         <v>3000</v>
       </c>
-      <c r="G9" t="s"/>
-      <c r="H9" t="n">
+      <c t="s" r="G9"/>
+      <c t="n" r="H9">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" t="n">
+      <c t="n" r="A10">
         <v>7839</v>
       </c>
-      <c r="B10" t="s">
+      <c t="s" r="B10">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c t="s" r="C10">
         <v>30</v>
       </c>
-      <c r="D10" t="s"/>
-      <c r="E10" t="s">
+      <c t="s" r="D10"/>
+      <c t="s" r="E10">
         <v>31</v>
       </c>
-      <c r="F10" t="n">
+      <c t="n" r="F10">
         <v>5000</v>
       </c>
-      <c r="G10" t="s"/>
-      <c r="H10" t="n">
+      <c t="s" r="G10"/>
+      <c t="n" r="H10">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" t="n">
+      <c t="n" r="A11">
         <v>7876</v>
       </c>
-      <c r="B11" t="s">
+      <c t="s" r="B11">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c t="s" r="C11">
         <v>33</v>
       </c>
-      <c r="D11" t="n">
+      <c t="n" r="D11">
         <v>7788</v>
       </c>
-      <c r="E11" t="s">
+      <c t="s" r="E11">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
+      <c t="s" r="F11">
         <v>35</v>
       </c>
-      <c r="G11" t="s"/>
-      <c r="H11" t="n">
+      <c t="s" r="G11"/>
+      <c t="n" r="H11">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" t="n">
+      <c t="n" r="A12">
         <v>7900</v>
       </c>
-      <c r="B12" t="s">
+      <c t="s" r="B12">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c t="s" r="C12">
         <v>33</v>
       </c>
-      <c r="D12" t="n">
+      <c t="n" r="D12">
         <v>7698</v>
       </c>
-      <c r="E12" t="s">
+      <c t="s" r="E12">
         <v>37</v>
       </c>
-      <c r="F12" t="n">
+      <c t="n" r="F12">
         <v>950</v>
       </c>
-      <c r="G12" t="s"/>
-      <c r="H12" t="n">
+      <c t="s" r="G12"/>
+      <c t="n" r="H12">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" t="n">
+      <c t="n" r="A13">
         <v>7902</v>
       </c>
-      <c r="B13" t="s">
+      <c t="s" r="B13">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c t="s" r="C13">
         <v>27</v>
       </c>
-      <c r="D13" t="n">
+      <c t="n" r="D13">
         <v>7566</v>
       </c>
-      <c r="E13" t="s">
+      <c t="s" r="E13">
         <v>37</v>
       </c>
-      <c r="F13" t="n">
+      <c t="n" r="F13">
         <v>3000</v>
       </c>
-      <c r="G13" t="s"/>
-      <c r="H13" t="n">
+      <c t="s" r="G13"/>
+      <c t="n" r="H13">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add namespace attribute to schemas
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -494,321 +494,321 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c t="s" r="A1">
+    <row spans="1:8" r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c t="n" r="A2">
+    <row spans="1:8" r="2">
+      <c r="A2" t="n">
         <v>7369</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c t="n" r="D2">
+      <c r="D2" t="n">
         <v>7902</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c t="n" r="F2">
+      <c r="F2" t="n">
         <v>800</v>
       </c>
-      <c t="s" r="G2"/>
-      <c t="n" r="H2">
+      <c r="G2" t="s"/>
+      <c r="H2" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c t="n" r="A3">
+    <row spans="1:8" r="3">
+      <c r="A3" t="n">
         <v>7499</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="C3">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c t="n" r="D3">
+      <c r="D3" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E3">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c t="n" r="F3">
+      <c r="F3" t="n">
         <v>1600</v>
       </c>
-      <c t="n" r="G3">
+      <c r="G3" t="n">
         <v>300</v>
       </c>
-      <c t="n" r="H3">
+      <c r="H3" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c t="n" r="A4">
+    <row spans="1:8" r="4">
+      <c r="A4" t="n">
         <v>7521</v>
       </c>
-      <c t="s" r="B4">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c t="n" r="D4">
+      <c r="D4" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E4">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="F4">
+      <c r="F4" t="n">
         <v>1250</v>
       </c>
-      <c t="n" r="G4">
+      <c r="G4" t="n">
         <v>500</v>
       </c>
-      <c t="n" r="H4">
+      <c r="H4" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c t="n" r="A5">
+    <row spans="1:8" r="5">
+      <c r="A5" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D5">
+      <c r="D5" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E5">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c t="n" r="F5">
+      <c r="F5" t="n">
         <v>2975</v>
       </c>
-      <c t="s" r="G5"/>
-      <c t="n" r="H5">
+      <c r="G5" t="s"/>
+      <c r="H5" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c t="n" r="A6">
+    <row spans="1:8" r="6">
+      <c r="A6" t="n">
         <v>7654</v>
       </c>
-      <c t="s" r="B6">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="C6">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c t="n" r="D6">
+      <c r="D6" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E6">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c t="n" r="F6">
+      <c r="F6" t="n">
         <v>1250</v>
       </c>
-      <c t="n" r="G6">
+      <c r="G6" t="n">
         <v>1400</v>
       </c>
-      <c t="n" r="H6">
+      <c r="H6" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c t="n" r="A7">
+    <row spans="1:8" r="7">
+      <c r="A7" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D7">
+      <c r="D7" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E7">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c t="n" r="F7">
+      <c r="F7" t="n">
         <v>2850</v>
       </c>
-      <c t="s" r="G7"/>
-      <c t="n" r="H7">
+      <c r="G7" t="s"/>
+      <c r="H7" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c t="n" r="A8">
+    <row spans="1:8" r="8">
+      <c r="A8" t="n">
         <v>7782</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D8">
+      <c r="D8" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E8">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c t="n" r="F8">
+      <c r="F8" t="n">
         <v>2450</v>
       </c>
-      <c t="s" r="G8"/>
-      <c t="n" r="H8">
+      <c r="G8" t="s"/>
+      <c r="H8" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c t="n" r="A9">
+    <row spans="1:8" r="9">
+      <c r="A9" t="n">
         <v>7788</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c t="n" r="D9">
+      <c r="D9" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="E9">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c t="n" r="F9">
+      <c r="F9" t="n">
         <v>3000</v>
       </c>
-      <c t="s" r="G9"/>
-      <c t="n" r="H9">
+      <c r="G9" t="s"/>
+      <c r="H9" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c t="n" r="A10">
+    <row spans="1:8" r="10">
+      <c r="A10" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="D10"/>
-      <c t="s" r="E10">
+      <c r="D10" t="s"/>
+      <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c t="n" r="F10">
+      <c r="F10" t="n">
         <v>5000</v>
       </c>
-      <c t="s" r="G10"/>
-      <c t="n" r="H10">
+      <c r="G10" t="s"/>
+      <c r="H10" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c t="n" r="A11">
+    <row spans="1:8" r="11">
+      <c r="A11" t="n">
         <v>7876</v>
       </c>
-      <c t="s" r="B11">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c t="n" r="D11">
+      <c r="D11" t="n">
         <v>7788</v>
       </c>
-      <c t="s" r="E11">
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="F11">
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c t="s" r="G11"/>
-      <c t="n" r="H11">
+      <c r="G11" t="s"/>
+      <c r="H11" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c t="n" r="A12">
+    <row spans="1:8" r="12">
+      <c r="A12" t="n">
         <v>7900</v>
       </c>
-      <c t="s" r="B12">
+      <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c t="n" r="D12">
+      <c r="D12" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E12">
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c t="n" r="F12">
+      <c r="F12" t="n">
         <v>950</v>
       </c>
-      <c t="s" r="G12"/>
-      <c t="n" r="H12">
+      <c r="G12" t="s"/>
+      <c r="H12" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c t="n" r="A13">
+    <row spans="1:8" r="13">
+      <c r="A13" t="n">
         <v>7902</v>
       </c>
-      <c t="s" r="B13">
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="C13">
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c t="n" r="D13">
+      <c r="D13" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="E13">
+      <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c t="n" r="F13">
+      <c r="F13" t="n">
         <v>3000</v>
       </c>
-      <c t="s" r="G13"/>
-      <c t="n" r="H13">
+      <c r="G13" t="s"/>
+      <c r="H13" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move process into plug-in
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -495,320 +495,320 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row spans="1:8" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>7</v>
       </c>
     </row>
     <row spans="1:8" r="2">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>7369</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>9</v>
       </c>
-      <c r="D2" t="n">
+      <c t="n" r="D2">
         <v>7902</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>10</v>
       </c>
-      <c r="F2" t="n">
+      <c t="n" r="F2">
         <v>800</v>
       </c>
-      <c r="G2" t="s"/>
-      <c r="H2" t="n">
+      <c t="s" r="G2"/>
+      <c t="n" r="H2">
         <v>20</v>
       </c>
     </row>
     <row spans="1:8" r="3">
-      <c r="A3" t="n">
+      <c t="n" r="A3">
         <v>7499</v>
       </c>
-      <c r="B3" t="s">
+      <c t="s" r="B3">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c t="s" r="C3">
         <v>12</v>
       </c>
-      <c r="D3" t="n">
+      <c t="n" r="D3">
         <v>7698</v>
       </c>
-      <c r="E3" t="s">
+      <c t="s" r="E3">
         <v>13</v>
       </c>
-      <c r="F3" t="n">
+      <c t="n" r="F3">
         <v>1600</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>300</v>
       </c>
-      <c r="H3" t="n">
+      <c t="n" r="H3">
         <v>30</v>
       </c>
     </row>
     <row spans="1:8" r="4">
-      <c r="A4" t="n">
+      <c t="n" r="A4">
         <v>7521</v>
       </c>
-      <c r="B4" t="s">
+      <c t="s" r="B4">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c t="s" r="C4">
         <v>15</v>
       </c>
-      <c r="D4" t="n">
+      <c t="n" r="D4">
         <v>7698</v>
       </c>
-      <c r="E4" t="s">
+      <c t="s" r="E4">
         <v>16</v>
       </c>
-      <c r="F4" t="n">
+      <c t="n" r="F4">
         <v>1250</v>
       </c>
-      <c r="G4" t="n">
+      <c t="n" r="G4">
         <v>500</v>
       </c>
-      <c r="H4" t="n">
+      <c t="n" r="H4">
         <v>30</v>
       </c>
     </row>
     <row spans="1:8" r="5">
-      <c r="A5" t="n">
+      <c t="n" r="A5">
         <v>7566</v>
       </c>
-      <c r="B5" t="s">
+      <c t="s" r="B5">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c t="s" r="C5">
         <v>18</v>
       </c>
-      <c r="D5" t="n">
+      <c t="n" r="D5">
         <v>7839</v>
       </c>
-      <c r="E5" t="s">
+      <c t="s" r="E5">
         <v>19</v>
       </c>
-      <c r="F5" t="n">
+      <c t="n" r="F5">
         <v>2975</v>
       </c>
-      <c r="G5" t="s"/>
-      <c r="H5" t="n">
+      <c t="s" r="G5"/>
+      <c t="n" r="H5">
         <v>20</v>
       </c>
     </row>
     <row spans="1:8" r="6">
-      <c r="A6" t="n">
+      <c t="n" r="A6">
         <v>7654</v>
       </c>
-      <c r="B6" t="s">
+      <c t="s" r="B6">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c t="s" r="C6">
         <v>15</v>
       </c>
-      <c r="D6" t="n">
+      <c t="n" r="D6">
         <v>7698</v>
       </c>
-      <c r="E6" t="s">
+      <c t="s" r="E6">
         <v>21</v>
       </c>
-      <c r="F6" t="n">
+      <c t="n" r="F6">
         <v>1250</v>
       </c>
-      <c r="G6" t="n">
+      <c t="n" r="G6">
         <v>1400</v>
       </c>
-      <c r="H6" t="n">
+      <c t="n" r="H6">
         <v>30</v>
       </c>
     </row>
     <row spans="1:8" r="7">
-      <c r="A7" t="n">
+      <c t="n" r="A7">
         <v>7698</v>
       </c>
-      <c r="B7" t="s">
+      <c t="s" r="B7">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c t="s" r="C7">
         <v>18</v>
       </c>
-      <c r="D7" t="n">
+      <c t="n" r="D7">
         <v>7839</v>
       </c>
-      <c r="E7" t="s">
+      <c t="s" r="E7">
         <v>23</v>
       </c>
-      <c r="F7" t="n">
+      <c t="n" r="F7">
         <v>2850</v>
       </c>
-      <c r="G7" t="s"/>
-      <c r="H7" t="n">
+      <c t="s" r="G7"/>
+      <c t="n" r="H7">
         <v>30</v>
       </c>
     </row>
     <row spans="1:8" r="8">
-      <c r="A8" t="n">
+      <c t="n" r="A8">
         <v>7782</v>
       </c>
-      <c r="B8" t="s">
+      <c t="s" r="B8">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c t="s" r="C8">
         <v>18</v>
       </c>
-      <c r="D8" t="n">
+      <c t="n" r="D8">
         <v>7839</v>
       </c>
-      <c r="E8" t="s">
+      <c t="s" r="E8">
         <v>25</v>
       </c>
-      <c r="F8" t="n">
+      <c t="n" r="F8">
         <v>2450</v>
       </c>
-      <c r="G8" t="s"/>
-      <c r="H8" t="n">
+      <c t="s" r="G8"/>
+      <c t="n" r="H8">
         <v>10</v>
       </c>
     </row>
     <row spans="1:8" r="9">
-      <c r="A9" t="n">
+      <c t="n" r="A9">
         <v>7788</v>
       </c>
-      <c r="B9" t="s">
+      <c t="s" r="B9">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c t="s" r="C9">
         <v>27</v>
       </c>
-      <c r="D9" t="n">
+      <c t="n" r="D9">
         <v>7566</v>
       </c>
-      <c r="E9" t="s">
+      <c t="s" r="E9">
         <v>28</v>
       </c>
-      <c r="F9" t="n">
+      <c t="n" r="F9">
         <v>3000</v>
       </c>
-      <c r="G9" t="s"/>
-      <c r="H9" t="n">
+      <c t="s" r="G9"/>
+      <c t="n" r="H9">
         <v>20</v>
       </c>
     </row>
     <row spans="1:8" r="10">
-      <c r="A10" t="n">
+      <c t="n" r="A10">
         <v>7839</v>
       </c>
-      <c r="B10" t="s">
+      <c t="s" r="B10">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c t="s" r="C10">
         <v>30</v>
       </c>
-      <c r="D10" t="s"/>
-      <c r="E10" t="s">
+      <c t="s" r="D10"/>
+      <c t="s" r="E10">
         <v>31</v>
       </c>
-      <c r="F10" t="n">
+      <c t="n" r="F10">
         <v>5000</v>
       </c>
-      <c r="G10" t="s"/>
-      <c r="H10" t="n">
+      <c t="s" r="G10"/>
+      <c t="n" r="H10">
         <v>10</v>
       </c>
     </row>
     <row spans="1:8" r="11">
-      <c r="A11" t="n">
+      <c t="n" r="A11">
         <v>7876</v>
       </c>
-      <c r="B11" t="s">
+      <c t="s" r="B11">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c t="s" r="C11">
         <v>33</v>
       </c>
-      <c r="D11" t="n">
+      <c t="n" r="D11">
         <v>7788</v>
       </c>
-      <c r="E11" t="s">
+      <c t="s" r="E11">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
+      <c t="s" r="F11">
         <v>35</v>
       </c>
-      <c r="G11" t="s"/>
-      <c r="H11" t="n">
+      <c t="s" r="G11"/>
+      <c t="n" r="H11">
         <v>20</v>
       </c>
     </row>
     <row spans="1:8" r="12">
-      <c r="A12" t="n">
+      <c t="n" r="A12">
         <v>7900</v>
       </c>
-      <c r="B12" t="s">
+      <c t="s" r="B12">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c t="s" r="C12">
         <v>33</v>
       </c>
-      <c r="D12" t="n">
+      <c t="n" r="D12">
         <v>7698</v>
       </c>
-      <c r="E12" t="s">
+      <c t="s" r="E12">
         <v>37</v>
       </c>
-      <c r="F12" t="n">
+      <c t="n" r="F12">
         <v>950</v>
       </c>
-      <c r="G12" t="s"/>
-      <c r="H12" t="n">
+      <c t="s" r="G12"/>
+      <c t="n" r="H12">
         <v>30</v>
       </c>
     </row>
     <row spans="1:8" r="13">
-      <c r="A13" t="n">
+      <c t="n" r="A13">
         <v>7902</v>
       </c>
-      <c r="B13" t="s">
+      <c t="s" r="B13">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c t="s" r="C13">
         <v>27</v>
       </c>
-      <c r="D13" t="n">
+      <c t="n" r="D13">
         <v>7566</v>
       </c>
-      <c r="E13" t="s">
+      <c t="s" r="E13">
         <v>37</v>
       </c>
-      <c r="F13" t="n">
+      <c t="n" r="F13">
         <v>3000</v>
       </c>
-      <c r="G13" t="s"/>
-      <c r="H13" t="n">
+      <c t="s" r="G13"/>
+      <c t="n" r="H13">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add the SQLLite database type Do not use offsets, instead change compare-files
</commit_message>
<xml_diff>
--- a/qal/dataset/tests/resources/excel_out.xlsx
+++ b/qal/dataset/tests/resources/excel_out.xlsx
@@ -172,7 +172,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-    <s:pageSetUpPr/>
-  </s:sheetPr>
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -482,10 +482,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-    <s:pageSetUpPr/>
-  </s:sheetPr>
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -494,321 +494,321 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row spans="1:8" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row spans="1:8" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:8">
+      <c r="A2" t="n">
         <v>7369</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c t="n" r="D2">
+      <c r="D2" t="n">
         <v>7902</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c t="n" r="F2">
+      <c r="F2" t="n">
         <v>800</v>
       </c>
-      <c t="s" r="G2"/>
-      <c t="n" r="H2">
+      <c r="G2" t="s"/>
+      <c r="H2" t="n">
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:8">
+      <c r="A3" t="n">
         <v>7499</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="C3">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c t="n" r="D3">
+      <c r="D3" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E3">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c t="n" r="F3">
+      <c r="F3" t="n">
         <v>1600</v>
       </c>
-      <c t="n" r="G3">
+      <c r="G3" t="n">
         <v>300</v>
       </c>
-      <c t="n" r="H3">
+      <c r="H3" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="4">
-      <c t="n" r="A4">
+    <row r="4" spans="1:8">
+      <c r="A4" t="n">
         <v>7521</v>
       </c>
-      <c t="s" r="B4">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c t="n" r="D4">
+      <c r="D4" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E4">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="F4">
+      <c r="F4" t="n">
         <v>1250</v>
       </c>
-      <c t="n" r="G4">
+      <c r="G4" t="n">
         <v>500</v>
       </c>
-      <c t="n" r="H4">
+      <c r="H4" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="5">
-      <c t="n" r="A5">
+    <row r="5" spans="1:8">
+      <c r="A5" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D5">
+      <c r="D5" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E5">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c t="n" r="F5">
+      <c r="F5" t="n">
         <v>2975</v>
       </c>
-      <c t="s" r="G5"/>
-      <c t="n" r="H5">
+      <c r="G5" t="s"/>
+      <c r="H5" t="n">
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="6">
-      <c t="n" r="A6">
+    <row r="6" spans="1:8">
+      <c r="A6" t="n">
         <v>7654</v>
       </c>
-      <c t="s" r="B6">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="C6">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c t="n" r="D6">
+      <c r="D6" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E6">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c t="n" r="F6">
+      <c r="F6" t="n">
         <v>1250</v>
       </c>
-      <c t="n" r="G6">
+      <c r="G6" t="n">
         <v>1400</v>
       </c>
-      <c t="n" r="H6">
+      <c r="H6" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="7">
-      <c t="n" r="A7">
+    <row r="7" spans="1:8">
+      <c r="A7" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D7">
+      <c r="D7" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E7">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c t="n" r="F7">
+      <c r="F7" t="n">
         <v>2850</v>
       </c>
-      <c t="s" r="G7"/>
-      <c t="n" r="H7">
+      <c r="G7" t="s"/>
+      <c r="H7" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="8">
-      <c t="n" r="A8">
+    <row r="8" spans="1:8">
+      <c r="A8" t="n">
         <v>7782</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="D8">
+      <c r="D8" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="E8">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c t="n" r="F8">
+      <c r="F8" t="n">
         <v>2450</v>
       </c>
-      <c t="s" r="G8"/>
-      <c t="n" r="H8">
+      <c r="G8" t="s"/>
+      <c r="H8" t="n">
         <v>10</v>
       </c>
     </row>
-    <row spans="1:8" r="9">
-      <c t="n" r="A9">
+    <row r="9" spans="1:8">
+      <c r="A9" t="n">
         <v>7788</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c t="n" r="D9">
+      <c r="D9" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="E9">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c t="n" r="F9">
+      <c r="F9" t="n">
         <v>3000</v>
       </c>
-      <c t="s" r="G9"/>
-      <c t="n" r="H9">
+      <c r="G9" t="s"/>
+      <c r="H9" t="n">
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="10">
-      <c t="n" r="A10">
+    <row r="10" spans="1:8">
+      <c r="A10" t="n">
         <v>7839</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="D10"/>
-      <c t="s" r="E10">
+      <c r="D10" t="s"/>
+      <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c t="n" r="F10">
+      <c r="F10" t="n">
         <v>5000</v>
       </c>
-      <c t="s" r="G10"/>
-      <c t="n" r="H10">
+      <c r="G10" t="s"/>
+      <c r="H10" t="n">
         <v>10</v>
       </c>
     </row>
-    <row spans="1:8" r="11">
-      <c t="n" r="A11">
+    <row r="11" spans="1:8">
+      <c r="A11" t="n">
         <v>7876</v>
       </c>
-      <c t="s" r="B11">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c t="n" r="D11">
+      <c r="D11" t="n">
         <v>7788</v>
       </c>
-      <c t="s" r="E11">
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="F11">
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c t="s" r="G11"/>
-      <c t="n" r="H11">
+      <c r="G11" t="s"/>
+      <c r="H11" t="n">
         <v>20</v>
       </c>
     </row>
-    <row spans="1:8" r="12">
-      <c t="n" r="A12">
+    <row r="12" spans="1:8">
+      <c r="A12" t="n">
         <v>7900</v>
       </c>
-      <c t="s" r="B12">
+      <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c t="n" r="D12">
+      <c r="D12" t="n">
         <v>7698</v>
       </c>
-      <c t="s" r="E12">
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c t="n" r="F12">
+      <c r="F12" t="n">
         <v>950</v>
       </c>
-      <c t="s" r="G12"/>
-      <c t="n" r="H12">
+      <c r="G12" t="s"/>
+      <c r="H12" t="n">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:8" r="13">
-      <c t="n" r="A13">
+    <row r="13" spans="1:8">
+      <c r="A13" t="n">
         <v>7902</v>
       </c>
-      <c t="s" r="B13">
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="C13">
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c t="n" r="D13">
+      <c r="D13" t="n">
         <v>7566</v>
       </c>
-      <c t="s" r="E13">
+      <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c t="n" r="F13">
+      <c r="F13" t="n">
         <v>3000</v>
       </c>
-      <c t="s" r="G13"/>
-      <c t="n" r="H13">
+      <c r="G13" t="s"/>
+      <c r="H13" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>